<commit_message>
GoodInfo_v2 - 2021-12-16 未完成
</commit_message>
<xml_diff>
--- a/TodayOpenPosition_2021-12-16.xlsx
+++ b/TodayOpenPosition_2021-12-16.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\TradingModel_v3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\GoodInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1080,16 +1080,16 @@
         <v>51.6</v>
       </c>
       <c r="F2">
-        <v>60.2</v>
+        <v>60.8</v>
       </c>
       <c r="G2">
-        <v>1739</v>
+        <v>1757</v>
       </c>
       <c r="H2">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="I2" s="1">
-        <v>0.16170000000000001</v>
+        <v>0.17369999999999999</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -1118,22 +1118,22 @@
         <v>265.5</v>
       </c>
       <c r="F3">
-        <v>275</v>
+        <v>282.5</v>
       </c>
       <c r="G3">
-        <v>1645</v>
+        <v>1689</v>
       </c>
       <c r="H3">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="I3" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>5.96E-2</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L3" t="s">
         <v>14</v>
@@ -1156,22 +1156,22 @@
         <v>68.91</v>
       </c>
       <c r="F4">
-        <v>83.5</v>
+        <v>81</v>
       </c>
       <c r="G4">
-        <v>3411</v>
+        <v>3310</v>
       </c>
       <c r="H4">
-        <v>584</v>
+        <v>483</v>
       </c>
       <c r="I4" s="1">
-        <v>0.20660000000000001</v>
+        <v>0.1709</v>
       </c>
       <c r="J4">
         <v>2</v>
       </c>
       <c r="K4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L4" t="s">
         <v>14</v>
@@ -1194,16 +1194,16 @@
         <v>211.5</v>
       </c>
       <c r="F5">
-        <v>221.5</v>
+        <v>225</v>
       </c>
       <c r="G5">
-        <v>1545</v>
+        <v>1570</v>
       </c>
       <c r="H5">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="I5" s="1">
-        <v>4.3200000000000002E-2</v>
+        <v>6.0100000000000001E-2</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -1232,16 +1232,16 @@
         <v>46.6</v>
       </c>
       <c r="F6">
-        <v>44.2</v>
+        <v>42.75</v>
       </c>
       <c r="G6">
-        <v>1409</v>
+        <v>1363</v>
       </c>
       <c r="H6">
-        <v>-83</v>
+        <v>-129</v>
       </c>
       <c r="I6" s="1">
-        <v>-5.5599999999999997E-2</v>
+        <v>-8.6499999999999994E-2</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -1270,16 +1270,16 @@
         <v>248</v>
       </c>
       <c r="F7">
-        <v>279.5</v>
+        <v>278</v>
       </c>
       <c r="G7">
-        <v>1671</v>
+        <v>1662</v>
       </c>
       <c r="H7">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="I7" s="1">
-        <v>0.1222</v>
+        <v>0.1162</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1308,16 +1308,16 @@
         <v>243.25</v>
       </c>
       <c r="F8">
-        <v>284.5</v>
+        <v>302</v>
       </c>
       <c r="G8">
-        <v>3402</v>
+        <v>3612</v>
       </c>
       <c r="H8">
-        <v>481</v>
+        <v>691</v>
       </c>
       <c r="I8" s="1">
-        <v>0.16470000000000001</v>
+        <v>0.2366</v>
       </c>
       <c r="J8">
         <v>2</v>
@@ -1346,16 +1346,16 @@
         <v>283.5</v>
       </c>
       <c r="F9">
-        <v>291</v>
+        <v>320</v>
       </c>
       <c r="G9">
-        <v>1450</v>
+        <v>1595</v>
       </c>
       <c r="H9">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="I9" s="1">
-        <v>2.2599999999999999E-2</v>
+        <v>0.12479999999999999</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -1384,16 +1384,16 @@
         <v>40</v>
       </c>
       <c r="F10">
-        <v>43.95</v>
+        <v>44.15</v>
       </c>
       <c r="G10">
-        <v>1621</v>
+        <v>1628</v>
       </c>
       <c r="H10">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="I10" s="1">
-        <v>9.4500000000000001E-2</v>
+        <v>9.9299999999999999E-2</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -1422,16 +1422,16 @@
         <v>170</v>
       </c>
       <c r="F11">
-        <v>189.5</v>
+        <v>208</v>
       </c>
       <c r="G11">
-        <v>1699</v>
+        <v>1866</v>
       </c>
       <c r="H11">
-        <v>168</v>
+        <v>335</v>
       </c>
       <c r="I11" s="1">
-        <v>0.10970000000000001</v>
+        <v>0.21879999999999999</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -1460,16 +1460,16 @@
         <v>17.399999999999999</v>
       </c>
       <c r="F12">
-        <v>17.75</v>
+        <v>17.55</v>
       </c>
       <c r="G12">
-        <v>1503</v>
+        <v>1486</v>
       </c>
       <c r="H12">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="I12" s="1">
-        <v>1.55E-2</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1498,16 +1498,16 @@
         <v>115.5</v>
       </c>
       <c r="F13">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="G13">
-        <v>1749</v>
+        <v>1853</v>
       </c>
       <c r="H13">
-        <v>247</v>
+        <v>351</v>
       </c>
       <c r="I13" s="1">
-        <v>0.16439999999999999</v>
+        <v>0.23369999999999999</v>
       </c>
       <c r="J13">
         <v>1</v>

</xml_diff>